<commit_message>
Implementing a project Petstore
</commit_message>
<xml_diff>
--- a/testData/ProjectName_TestData File.xlsx
+++ b/testData/ProjectName_TestData File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LinuVarghese\Documents\Selenium-Automation\AutomationFramework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF347F2-7211-4349-B8DE-0510623168B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEB7FC4-22C6-48B8-A3E8-71980C109D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A3B0D007-71D6-403B-B118-F5004725861B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{A3B0D007-71D6-403B-B118-F5004725861B}"/>
   </bookViews>
   <sheets>
     <sheet name="MainLogin" sheetId="2" r:id="rId1"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>